<commit_message>
Finalização do despertador, att do Taskboard.xlsx
</commit_message>
<xml_diff>
--- a/Documentos/RequisitosAnaliseProjeto/Royalt Hotel - Backlog Requirements.xlsx
+++ b/Documentos/RequisitosAnaliseProjeto/Royalt Hotel - Backlog Requirements.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="4815" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="4815"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Requisitos" sheetId="1" r:id="rId1"/>
@@ -405,11 +405,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="79747328"/>
-        <c:axId val="80089472"/>
+        <c:axId val="70203648"/>
+        <c:axId val="70230400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="79747328"/>
+        <c:axId val="70203648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -436,12 +436,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80089472"/>
+        <c:crossAx val="70230400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80089472"/>
+        <c:axId val="70230400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5100"/>
@@ -451,7 +451,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="79747328"/>
+        <c:crossAx val="70203648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -464,7 +464,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000047" footer="0.31496062000000047"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -618,11 +618,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="80114432"/>
-        <c:axId val="80116352"/>
+        <c:axId val="70243072"/>
+        <c:axId val="70244992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80114432"/>
+        <c:axId val="70243072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -649,12 +649,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80116352"/>
+        <c:crossAx val="70244992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80116352"/>
+        <c:axId val="70244992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -664,7 +664,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80114432"/>
+        <c:crossAx val="70243072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -677,7 +677,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000058" footer="0.31496062000000058"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2468,7 +2468,7 @@
   <dgm:whole/>
   <dgm:extLst>
     <a:ext uri="http://schemas.microsoft.com/office/drawing/2008/diagram">
-      <dsp:dataModelExt xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns="" relId="rId5" minVer="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+      <dsp:dataModelExt xmlns="" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" relId="rId5" minVer="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
     </a:ext>
   </dgm:extLst>
 </dgm:dataModel>
@@ -6170,8 +6170,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:AC295"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17944,7 +17944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Alterações no fim da sprint 3
</commit_message>
<xml_diff>
--- a/Documentos/RequisitosAnaliseProjeto/Royalt Hotel - Backlog Requirements.xlsx
+++ b/Documentos/RequisitosAnaliseProjeto/Royalt Hotel - Backlog Requirements.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="4815"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="4815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Requisitos" sheetId="1" r:id="rId1"/>
     <sheet name="Hierarquia dos Requisitos" sheetId="3" r:id="rId2"/>
     <sheet name="Gráficos" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Estórias</t>
   </si>
@@ -81,9 +81,6 @@
     <t>BV restante</t>
   </si>
   <si>
-    <t>BV restante planejado</t>
-  </si>
-  <si>
     <t>SP restante planejado</t>
   </si>
   <si>
@@ -95,14 +92,17 @@
   <si>
     <t>SP restante</t>
   </si>
+  <si>
+    <t>BV  planejado</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -209,7 +209,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -225,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -280,7 +280,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>Business Value restante</a:t>
+              <a:t>Burndown (Business Value)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -311,6 +311,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
@@ -342,7 +345,7 @@
                   <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>500</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -357,7 +360,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>BV restante planejado</c:v>
+                  <c:v>BV  planejado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -368,6 +371,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
@@ -405,11 +411,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="70203648"/>
-        <c:axId val="70230400"/>
+        <c:axId val="81356288"/>
+        <c:axId val="81358208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70203648"/>
+        <c:axId val="81356288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -436,12 +442,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70230400"/>
+        <c:crossAx val="81358208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70230400"/>
+        <c:axId val="81358208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5100"/>
@@ -451,7 +457,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70203648"/>
+        <c:crossAx val="81356288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -464,7 +470,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -524,6 +530,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
@@ -555,7 +564,7 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -581,6 +590,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
@@ -618,11 +630,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="70243072"/>
-        <c:axId val="70244992"/>
+        <c:axId val="81395712"/>
+        <c:axId val="81397632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70243072"/>
+        <c:axId val="81395712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -649,12 +661,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70244992"/>
+        <c:crossAx val="81397632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70244992"/>
+        <c:axId val="81397632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -664,7 +676,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70243072"/>
+        <c:crossAx val="81395712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -677,7 +689,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2472,1134 +2484,6 @@
     </a:ext>
   </dgm:extLst>
 </dgm:dataModel>
-</file>
-
-<file path=xl/diagrams/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram">
-  <dsp:spTree>
-    <dsp:nvGrpSpPr>
-      <dsp:cNvPr id="0" name=""/>
-      <dsp:cNvGrpSpPr/>
-    </dsp:nvGrpSpPr>
-    <dsp:grpSpPr/>
-    <dsp:sp modelId="{D7A28C4B-08F3-417C-9918-B9B56B5039D3}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="7855836" y="756203"/>
-          <a:ext cx="850351" cy="295163"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="0" y="147581"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="850351" y="147581"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="850351" y="295163"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{3A7EE58E-683E-4C02-A9CD-84660C7CC0F8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="7005485" y="756203"/>
-          <a:ext cx="850351" cy="295163"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="850351" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="850351" y="147581"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="147581"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="295163"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{561721DE-941D-4E73-AE63-1A5513B19025}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5239244" y="754762"/>
-          <a:ext cx="91440" cy="317834"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="45748" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="45748" y="170252"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="45720" y="170252"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="45720" y="317834"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{BF217FC9-F0DA-4FE4-B62F-FDED1529460F}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2299475" y="740404"/>
-          <a:ext cx="91440" cy="337919"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="72467" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="72467" y="190338"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="45720" y="190338"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="45720" y="337919"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{C2C4D24A-E9E2-424B-93EB-A6D50006AFE8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2371942" y="740404"/>
-          <a:ext cx="1439468" cy="342543"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="0" y="194962"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="1439468" y="194962"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="1439468" y="342543"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{4A2142FB-2972-4A64-8B0C-409EF09121F9}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="925924" y="740404"/>
-          <a:ext cx="1446018" cy="336183"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="1446018" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="1446018" y="188602"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="188602"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="336183"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{25A01E64-0E1F-4115-A47C-FBC8FF75B5EA}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="1669173" y="37635"/>
-          <a:ext cx="1405539" cy="702769"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>5(Recepcionista) Cadastro de reservas</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="1669173" y="37635"/>
-        <a:ext cx="1405539" cy="702769"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{744DEAA5-48C9-491B-A1CB-4DC74C87041E}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="223154" y="1076588"/>
-          <a:ext cx="1405539" cy="702769"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>6(Recepcionista) Cadastro de despertador</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="223154" y="1076588"/>
-        <a:ext cx="1405539" cy="702769"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{59514516-96D5-4A15-ADFB-8636BD4637F9}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3166227" y="1082948"/>
-          <a:ext cx="1290369" cy="702769"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>10(Gerente) Relatórios de hospedagem</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3166227" y="1082948"/>
-        <a:ext cx="1290369" cy="702769"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{3B641322-069C-4EB1-BA6C-01FE9202579F}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="1642425" y="1078324"/>
-          <a:ext cx="1405539" cy="702769"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>8(Recepcionista) Checkout e pagamento das reservas</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="1642425" y="1078324"/>
-        <a:ext cx="1405539" cy="702769"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{1E89CE54-0C6E-4873-A065-58E6EC22B713}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4582223" y="30762"/>
-          <a:ext cx="1405539" cy="724000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>2(Recepcionista) Cadastro de clientes</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4582223" y="30762"/>
-        <a:ext cx="1405539" cy="724000"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{CD95EC71-0A87-43ED-B13A-53400D8C62A4}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4582195" y="1072596"/>
-          <a:ext cx="1405539" cy="702769"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>3(Gerente) Cadastro e exclusão de clientes</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4582195" y="1072596"/>
-        <a:ext cx="1405539" cy="702769"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{91C48588-F4C1-48F4-A662-5F0AF538F0C5}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="7153066" y="53433"/>
-          <a:ext cx="1405539" cy="702769"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>4(Recepcionista) Cadastro de quarto</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="7153066" y="53433"/>
-        <a:ext cx="1405539" cy="702769"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{30E8178D-7B38-44E7-887B-24FAEF535DA8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="6302715" y="1051366"/>
-          <a:ext cx="1405539" cy="702769"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>1(Recepcionista) Quadro ocupação apartamentos</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="6302715" y="1051366"/>
-        <a:ext cx="1405539" cy="702769"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{4B53D9F5-1B77-441E-AAFB-AEF480B316A7}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="8003417" y="1051366"/>
-          <a:ext cx="1405539" cy="702769"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>7(Recepcionista) Controle de limpeza dos quartos</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="8003417" y="1051366"/>
-        <a:ext cx="1405539" cy="702769"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{D95422D7-13E1-41BE-AAE3-124F78F6B690}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="8904846" y="53433"/>
-          <a:ext cx="1405539" cy="702769"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
-            <a:t>9(Gerente) Configuração de senha</a:t>
-          </a:r>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="8904846" y="53433"/>
-        <a:ext cx="1405539" cy="702769"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-  </dsp:spTree>
-</dsp:drawing>
 </file>
 
 <file path=xl/diagrams/layout1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6170,8 +5054,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:AC295"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6194,10 +5078,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>14</v>
@@ -6515,9 +5399,7 @@
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="H8" s="10"/>
       <c r="I8" s="11"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -17944,8 +16826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17964,17 +16846,19 @@
         <v>20</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>25</v>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="12">
+        <v>0</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="12"/>
       <c r="B3" s="12">
         <v>5100</v>
       </c>
@@ -18027,13 +16911,13 @@
         <v>3</v>
       </c>
       <c r="B6" s="12">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="C6" s="13">
         <v>500</v>
       </c>
       <c r="D6" s="13">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" s="13">
         <v>8</v>

</xml_diff>

<commit_message>
Documentos atualizados da sprint4
</commit_message>
<xml_diff>
--- a/Documentos/RequisitosAnaliseProjeto/Royalt Hotel - Backlog Requirements.xlsx
+++ b/Documentos/RequisitosAnaliseProjeto/Royalt Hotel - Backlog Requirements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="4815" activeTab="2"/>
@@ -11,12 +11,12 @@
     <sheet name="Hierarquia dos Requisitos" sheetId="3" r:id="rId2"/>
     <sheet name="Gráficos" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Estórias</t>
   </si>
@@ -101,8 +101,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -209,7 +209,7 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -225,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -347,6 +347,9 @@
                 <c:pt idx="3">
                   <c:v>700</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -407,15 +410,18 @@
                 <c:pt idx="3">
                   <c:v>500</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="81356288"/>
-        <c:axId val="81358208"/>
+        <c:axId val="99307520"/>
+        <c:axId val="101428224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81356288"/>
+        <c:axId val="99307520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -442,12 +448,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81358208"/>
+        <c:crossAx val="101428224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81358208"/>
+        <c:axId val="101428224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5100"/>
@@ -457,7 +463,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81356288"/>
+        <c:crossAx val="99307520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -470,7 +476,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -566,6 +572,9 @@
                 <c:pt idx="3">
                   <c:v>10</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -626,15 +635,18 @@
                 <c:pt idx="3">
                   <c:v>8</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="81395712"/>
-        <c:axId val="81397632"/>
+        <c:axId val="101303808"/>
+        <c:axId val="101305728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81395712"/>
+        <c:axId val="101303808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -661,12 +673,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81397632"/>
+        <c:crossAx val="101305728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81397632"/>
+        <c:axId val="101305728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40"/>
@@ -676,7 +688,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81395712"/>
+        <c:crossAx val="101303808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -689,7 +701,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000091" footer="0.31496062000000091"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2480,10 +2492,1138 @@
   <dgm:whole/>
   <dgm:extLst>
     <a:ext uri="http://schemas.microsoft.com/office/drawing/2008/diagram">
-      <dsp:dataModelExt xmlns="" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" relId="rId5" minVer="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+      <dsp:dataModelExt xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns="" relId="rId5" minVer="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
     </a:ext>
   </dgm:extLst>
 </dgm:dataModel>
+</file>
+
+<file path=xl/diagrams/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram">
+  <dsp:spTree>
+    <dsp:nvGrpSpPr>
+      <dsp:cNvPr id="0" name=""/>
+      <dsp:cNvGrpSpPr/>
+    </dsp:nvGrpSpPr>
+    <dsp:grpSpPr/>
+    <dsp:sp modelId="{D7A28C4B-08F3-417C-9918-B9B56B5039D3}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7855836" y="756203"/>
+          <a:ext cx="850351" cy="295163"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="147581"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="850351" y="147581"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="850351" y="295163"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{3A7EE58E-683E-4C02-A9CD-84660C7CC0F8}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7005485" y="756203"/>
+          <a:ext cx="850351" cy="295163"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="850351" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="850351" y="147581"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="147581"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="295163"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{561721DE-941D-4E73-AE63-1A5513B19025}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5239244" y="754762"/>
+          <a:ext cx="91440" cy="317834"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="45748" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="45748" y="170252"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="45720" y="170252"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="45720" y="317834"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{BF217FC9-F0DA-4FE4-B62F-FDED1529460F}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2299475" y="740404"/>
+          <a:ext cx="91440" cy="337919"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="72467" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="72467" y="190338"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="45720" y="190338"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="45720" y="337919"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{C2C4D24A-E9E2-424B-93EB-A6D50006AFE8}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2371942" y="740404"/>
+          <a:ext cx="1439468" cy="342543"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="194962"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1439468" y="194962"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="1439468" y="342543"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{4A2142FB-2972-4A64-8B0C-409EF09121F9}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="925924" y="740404"/>
+          <a:ext cx="1446018" cy="336183"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="1446018" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="1446018" y="188602"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="188602"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="336183"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{25A01E64-0E1F-4115-A47C-FBC8FF75B5EA}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1669173" y="37635"/>
+          <a:ext cx="1405539" cy="702769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>5(Recepcionista) Cadastro de reservas</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="1669173" y="37635"/>
+        <a:ext cx="1405539" cy="702769"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{744DEAA5-48C9-491B-A1CB-4DC74C87041E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="223154" y="1076588"/>
+          <a:ext cx="1405539" cy="702769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>6(Recepcionista) Cadastro de despertador</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="223154" y="1076588"/>
+        <a:ext cx="1405539" cy="702769"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{59514516-96D5-4A15-ADFB-8636BD4637F9}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3166227" y="1082948"/>
+          <a:ext cx="1290369" cy="702769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>10(Gerente) Relatórios de hospedagem</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3166227" y="1082948"/>
+        <a:ext cx="1290369" cy="702769"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{3B641322-069C-4EB1-BA6C-01FE9202579F}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1642425" y="1078324"/>
+          <a:ext cx="1405539" cy="702769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>8(Recepcionista) Checkout e pagamento das reservas</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="1642425" y="1078324"/>
+        <a:ext cx="1405539" cy="702769"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{1E89CE54-0C6E-4873-A065-58E6EC22B713}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4582223" y="30762"/>
+          <a:ext cx="1405539" cy="724000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>2(Recepcionista) Cadastro de clientes</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4582223" y="30762"/>
+        <a:ext cx="1405539" cy="724000"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{CD95EC71-0A87-43ED-B13A-53400D8C62A4}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4582195" y="1072596"/>
+          <a:ext cx="1405539" cy="702769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>3(Gerente) Cadastro e exclusão de clientes</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4582195" y="1072596"/>
+        <a:ext cx="1405539" cy="702769"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{91C48588-F4C1-48F4-A662-5F0AF538F0C5}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="7153066" y="53433"/>
+          <a:ext cx="1405539" cy="702769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>4(Recepcionista) Cadastro de quarto</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="7153066" y="53433"/>
+        <a:ext cx="1405539" cy="702769"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{30E8178D-7B38-44E7-887B-24FAEF535DA8}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="6302715" y="1051366"/>
+          <a:ext cx="1405539" cy="702769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>1(Recepcionista) Quadro ocupação apartamentos</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="6302715" y="1051366"/>
+        <a:ext cx="1405539" cy="702769"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{4B53D9F5-1B77-441E-AAFB-AEF480B316A7}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="8003417" y="1051366"/>
+          <a:ext cx="1405539" cy="702769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>7(Recepcionista) Controle de limpeza dos quartos</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="8003417" y="1051366"/>
+        <a:ext cx="1405539" cy="702769"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{D95422D7-13E1-41BE-AAE3-124F78F6B690}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="8904846" y="53433"/>
+          <a:ext cx="1405539" cy="702769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="7620" tIns="7620" rIns="7620" bIns="7620" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="533400">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1200" kern="1200"/>
+            <a:t>9(Gerente) Configuração de senha</a:t>
+          </a:r>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="8904846" y="53433"/>
+        <a:ext cx="1405539" cy="702769"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+  </dsp:spTree>
+</dsp:drawing>
 </file>
 
 <file path=xl/diagrams/layout1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5054,9 +6194,7 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:AC295"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5400,7 +6538,9 @@
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
       <c r="H8" s="10"/>
-      <c r="I8" s="11"/>
+      <c r="I8" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -5530,7 +6670,9 @@
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="I11" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -16826,9 +17968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -16927,10 +18067,18 @@
       <c r="A7" s="12">
         <v>4</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="B7" s="12">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13">
+        <v>0</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>